<commit_message>
working on import/export - 2
</commit_message>
<xml_diff>
--- a/public/assets/excel/example.xlsx
+++ b/public/assets/excel/example.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="6">
   <si>
     <t>Empleado</t>
   </si>
@@ -357,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D52" sqref="D52:D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -411,30 +411,791 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="1"/>
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42785</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="1"/>
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42786</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42787</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="1"/>
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42788</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>42789</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="1"/>
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>42790</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="1"/>
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1">
+        <v>42791</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="1"/>
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>42792</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>42793</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>42794</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1">
+        <v>42795</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <v>42796</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1">
+        <v>42797</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1">
+        <v>42798</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1">
+        <v>42799</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1">
+        <v>42800</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1">
+        <v>42801</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1">
+        <v>42802</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1">
+        <v>42803</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1">
+        <v>42804</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1">
+        <v>42805</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1">
+        <v>42806</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1">
+        <v>42807</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1">
+        <v>42808</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="1">
+        <v>42809</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="1">
+        <v>42810</v>
+      </c>
+      <c r="C29">
+        <v>8</v>
+      </c>
+      <c r="D29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="1">
+        <v>42811</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="1">
+        <v>42812</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+      <c r="D31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="1">
+        <v>42813</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1">
+        <v>42814</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+      <c r="D33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1">
+        <v>42815</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1">
+        <v>42816</v>
+      </c>
+      <c r="C35">
+        <v>8</v>
+      </c>
+      <c r="D35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="1">
+        <v>42817</v>
+      </c>
+      <c r="C36">
+        <v>8</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="1">
+        <v>42818</v>
+      </c>
+      <c r="C37">
+        <v>8</v>
+      </c>
+      <c r="D37">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="1">
+        <v>42819</v>
+      </c>
+      <c r="C38">
+        <v>8</v>
+      </c>
+      <c r="D38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="1">
+        <v>42820</v>
+      </c>
+      <c r="C39">
+        <v>8</v>
+      </c>
+      <c r="D39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="1">
+        <v>42821</v>
+      </c>
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="D40">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="1">
+        <v>42822</v>
+      </c>
+      <c r="C41">
+        <v>8</v>
+      </c>
+      <c r="D41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="1">
+        <v>42823</v>
+      </c>
+      <c r="C42">
+        <v>8</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="1">
+        <v>42824</v>
+      </c>
+      <c r="C43">
+        <v>8</v>
+      </c>
+      <c r="D43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="1">
+        <v>42825</v>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="1">
+        <v>42826</v>
+      </c>
+      <c r="C45">
+        <v>8</v>
+      </c>
+      <c r="D45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="1">
+        <v>42827</v>
+      </c>
+      <c r="C46">
+        <v>8</v>
+      </c>
+      <c r="D46">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="1">
+        <v>42828</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="1">
+        <v>42829</v>
+      </c>
+      <c r="C48">
+        <v>8</v>
+      </c>
+      <c r="D48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="1">
+        <v>42830</v>
+      </c>
+      <c r="C49">
+        <v>8</v>
+      </c>
+      <c r="D49">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="1">
+        <v>42831</v>
+      </c>
+      <c r="C50">
+        <v>8</v>
+      </c>
+      <c r="D50">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="1">
+        <v>42832</v>
+      </c>
+      <c r="C51">
+        <v>8</v>
+      </c>
+      <c r="D51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="1">
+        <v>42833</v>
+      </c>
+      <c r="C52">
+        <v>8</v>
+      </c>
+      <c r="D52">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="1">
+        <v>42834</v>
+      </c>
+      <c r="C53">
+        <v>8</v>
+      </c>
+      <c r="D53">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="1">
+        <v>42835</v>
+      </c>
+      <c r="C54">
+        <v>8</v>
+      </c>
+      <c r="D54">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="1">
+        <v>42836</v>
+      </c>
+      <c r="C55">
+        <v>8</v>
+      </c>
+      <c r="D55">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="1">
+        <v>42837</v>
+      </c>
+      <c r="C56">
+        <v>8</v>
+      </c>
+      <c r="D56">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" s="1">
+        <v>42838</v>
+      </c>
+      <c r="C57">
+        <v>8</v>
+      </c>
+      <c r="D57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" s="1">
+        <v>42839</v>
+      </c>
+      <c r="C58">
+        <v>8</v>
+      </c>
+      <c r="D58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="1">
+        <v>42840</v>
+      </c>
+      <c r="C59">
+        <v>8</v>
+      </c>
+      <c r="D59">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated example imports file
</commit_message>
<xml_diff>
--- a/public/assets/excel/example.xlsx
+++ b/public/assets/excel/example.xlsx
@@ -366,7 +366,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B2" sqref="B2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -393,7 +393,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>42783</v>
+        <v>42811</v>
       </c>
       <c r="C2">
         <v>8</v>
@@ -407,7 +407,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>42784</v>
+        <v>42812</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -421,7 +421,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>42785</v>
+        <v>42813</v>
       </c>
       <c r="C4">
         <v>8</v>
@@ -435,7 +435,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>42786</v>
+        <v>42814</v>
       </c>
       <c r="C5">
         <v>8</v>
@@ -449,7 +449,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>42783</v>
+        <v>42815</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -463,7 +463,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>42784</v>
+        <v>42816</v>
       </c>
       <c r="C7">
         <v>8</v>
@@ -477,7 +477,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>42785</v>
+        <v>42817</v>
       </c>
       <c r="C8">
         <v>8</v>
@@ -491,7 +491,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1">
-        <v>42787</v>
+        <v>42818</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -505,7 +505,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="1">
-        <v>42783</v>
+        <v>42819</v>
       </c>
       <c r="C10">
         <v>8</v>

</xml_diff>